<commit_message>
cleaned up extracted columns e.g Accounting to Accountant for consistency and for easy sorting
</commit_message>
<xml_diff>
--- a/fertility_occupation.xlsx
+++ b/fertility_occupation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="376">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="369">
   <si>
     <t>MP</t>
   </si>
@@ -494,6 +494,9 @@
     <t>Enoch Teye Mensah</t>
   </si>
   <si>
+    <t>Edwin Nii Lantey Vanderpuye</t>
+  </si>
+  <si>
     <t>Patrick Yaw Boamah</t>
   </si>
   <si>
@@ -1112,46 +1115,22 @@
     <t>Kids</t>
   </si>
   <si>
-    <t>Edwin NiiŒæLantey Vanderpuye</t>
-  </si>
-  <si>
-    <t>business man"""business man""""</t>
-  </si>
-  <si>
-    <t>biochemist</t>
-  </si>
-  <si>
-    <t>farmer</t>
-  </si>
-  <si>
-    <t>Account Officer</t>
-  </si>
-  <si>
-    <t>Human Resource Manager</t>
-  </si>
-  <si>
-    <t>Marketing Expert</t>
-  </si>
-  <si>
-    <t>Farmer/Agriculturist</t>
-  </si>
-  <si>
-    <t>Head Teacher</t>
-  </si>
-  <si>
-    <t>Teaching</t>
-  </si>
-  <si>
-    <t>Tutor</t>
-  </si>
-  <si>
-    <t>Marketer</t>
-  </si>
-  <si>
-    <t>Project Planning</t>
-  </si>
-  <si>
-    <t>HR</t>
+    <t>Biochemist</t>
+  </si>
+  <si>
+    <t>I changed some occupation names like Accounting, Teaching etc. for conformity</t>
+  </si>
+  <si>
+    <t>I could have extracted the columns straight using R but I had to pull out occupation column and edit it first to enable consistency</t>
+  </si>
+  <si>
+    <t>Reason for Changes:</t>
+  </si>
+  <si>
+    <t>Changes:</t>
+  </si>
+  <si>
+    <t>I also replaced N/A with 0 for MPs who had N/A for number of kids</t>
   </si>
 </sst>
 </file>
@@ -1213,6 +1192,21 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:C276" totalsRowShown="0">
+  <autoFilter ref="A1:C276"/>
+  <sortState ref="A2:C276">
+    <sortCondition ref="B1:B276"/>
+  </sortState>
+  <tableColumns count="3">
+    <tableColumn id="1" name="MP"/>
+    <tableColumn id="2" name="Occupation"/>
+    <tableColumn id="3" name="Kids"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1512,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F276"/>
+  <dimension ref="A1:H276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,268 +1518,281 @@
     <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>207</v>
       </c>
       <c r="B2" t="s">
-        <v>275</v>
+        <v>343</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>301</v>
       </c>
       <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="H3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>301</v>
       </c>
       <c r="C4">
-        <v>4</v>
-      </c>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="G4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G5" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B6" t="s">
+        <v>301</v>
+      </c>
+      <c r="C6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>279</v>
-      </c>
-      <c r="C6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>279</v>
+        <v>301</v>
       </c>
       <c r="C8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c r="C10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>282</v>
+        <v>301</v>
       </c>
       <c r="C11">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="C12">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>281</v>
+        <v>301</v>
       </c>
       <c r="C13">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>255</v>
       </c>
       <c r="B14" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="C14">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>256</v>
       </c>
       <c r="B15" t="s">
-        <v>285</v>
+        <v>301</v>
       </c>
       <c r="C15">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>270</v>
       </c>
       <c r="B16" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="C16">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>287</v>
+        <v>352</v>
       </c>
       <c r="C17">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>288</v>
+        <v>335</v>
       </c>
       <c r="C18">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>275</v>
+        <v>293</v>
       </c>
       <c r="C20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>147</v>
       </c>
       <c r="B21" t="s">
-        <v>290</v>
+        <v>327</v>
       </c>
       <c r="C21">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>285</v>
+        <v>310</v>
       </c>
       <c r="C22">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>127</v>
       </c>
       <c r="B23" t="s">
-        <v>275</v>
+        <v>310</v>
       </c>
       <c r="C23">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>291</v>
+        <v>310</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1793,21 +1800,21 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>234</v>
       </c>
       <c r="B25" t="s">
-        <v>278</v>
+        <v>310</v>
       </c>
       <c r="C25">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>262</v>
       </c>
       <c r="B26" t="s">
-        <v>292</v>
+        <v>356</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1815,10 +1822,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1826,120 +1833,120 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>214</v>
       </c>
       <c r="B28" t="s">
-        <v>279</v>
+        <v>311</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C29">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="C30">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>291</v>
+        <v>285</v>
       </c>
       <c r="C31">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C32">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="C34">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="C35">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>158</v>
       </c>
       <c r="B36" t="s">
-        <v>277</v>
+        <v>285</v>
       </c>
       <c r="C36">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>296</v>
+        <v>277</v>
       </c>
       <c r="C37">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>286</v>
+        <v>363</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1947,32 +1954,32 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>272</v>
       </c>
       <c r="B39" t="s">
-        <v>298</v>
+        <v>360</v>
       </c>
       <c r="C39">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C40">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1980,24 +1987,24 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="C42">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C43">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
@@ -2005,7 +2012,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -2013,65 +2020,65 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C46">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C47">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C48">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="C49">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -2079,10 +2086,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>297</v>
+        <v>279</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -2090,43 +2097,43 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>297</v>
+        <v>324</v>
       </c>
       <c r="C52">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>139</v>
       </c>
       <c r="B53" t="s">
         <v>279</v>
       </c>
       <c r="C53">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>53</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>278</v>
+        <v>324</v>
       </c>
       <c r="C54">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>54</v>
+        <v>195</v>
       </c>
       <c r="B55" t="s">
-        <v>296</v>
+        <v>324</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -2134,65 +2141,65 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>248</v>
       </c>
       <c r="B56" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="C56">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>56</v>
+        <v>257</v>
       </c>
       <c r="B57" t="s">
-        <v>300</v>
+        <v>279</v>
       </c>
       <c r="C57">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>57</v>
+        <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>233</v>
       </c>
       <c r="B59" t="s">
-        <v>302</v>
+        <v>351</v>
       </c>
       <c r="C59">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>59</v>
+        <v>237</v>
       </c>
       <c r="B60" t="s">
-        <v>297</v>
+        <v>351</v>
       </c>
       <c r="C60">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>60</v>
+        <v>221</v>
       </c>
       <c r="B61" t="s">
-        <v>303</v>
+        <v>345</v>
       </c>
       <c r="C61">
         <v>3</v>
@@ -2200,32 +2207,32 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>279</v>
+        <v>292</v>
       </c>
       <c r="C62">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>62</v>
+        <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="C63">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>63</v>
+        <v>201</v>
       </c>
       <c r="B64" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="C64">
         <v>6</v>
@@ -2233,76 +2240,76 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>264</v>
       </c>
       <c r="B65" t="s">
-        <v>303</v>
+        <v>357</v>
       </c>
       <c r="C65">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>65</v>
+        <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C66">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>128</v>
       </c>
       <c r="B67" t="s">
-        <v>288</v>
+        <v>318</v>
       </c>
       <c r="C67">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="C68">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>68</v>
+        <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>305</v>
+        <v>315</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>69</v>
+        <v>227</v>
       </c>
       <c r="B70" t="s">
-        <v>275</v>
+        <v>348</v>
       </c>
       <c r="C70">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>284</v>
+        <v>325</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -2310,54 +2317,54 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>71</v>
+        <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C72">
-        <v>12</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>72</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>306</v>
+        <v>282</v>
       </c>
       <c r="C73">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>307</v>
+        <v>282</v>
       </c>
       <c r="C74">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>74</v>
+        <v>220</v>
       </c>
       <c r="B75" t="s">
-        <v>300</v>
+        <v>282</v>
       </c>
       <c r="C75">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>75</v>
+        <v>235</v>
       </c>
       <c r="B76" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -2365,384 +2372,384 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>76</v>
+        <v>132</v>
       </c>
       <c r="B77" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
       <c r="C77">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C78">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>78</v>
+        <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>278</v>
+        <v>286</v>
       </c>
       <c r="C79">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>275</v>
+        <v>286</v>
       </c>
       <c r="C80">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>80</v>
+        <v>44</v>
       </c>
       <c r="B81" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="C81">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="B82" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C82">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C83">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>124</v>
       </c>
       <c r="B84" t="s">
-        <v>363</v>
+        <v>286</v>
       </c>
       <c r="C84">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>84</v>
+        <v>249</v>
       </c>
       <c r="B85" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="C85">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>85</v>
+        <v>252</v>
       </c>
       <c r="B86" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C86">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>86</v>
+        <v>229</v>
       </c>
       <c r="B87" t="s">
-        <v>275</v>
+        <v>349</v>
       </c>
       <c r="C87">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>87</v>
+        <v>193</v>
       </c>
       <c r="B88" t="s">
-        <v>275</v>
+        <v>339</v>
       </c>
       <c r="C88">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>88</v>
+        <v>198</v>
       </c>
       <c r="B89" t="s">
-        <v>284</v>
+        <v>340</v>
       </c>
       <c r="C89">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>89</v>
+        <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="C90">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>309</v>
+        <v>280</v>
       </c>
       <c r="C91">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>91</v>
+        <v>27</v>
       </c>
       <c r="B92" t="s">
-        <v>310</v>
+        <v>280</v>
       </c>
       <c r="C92">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C93">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>93</v>
+        <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="C94">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>94</v>
+        <v>67</v>
       </c>
       <c r="B95" t="s">
-        <v>311</v>
+        <v>280</v>
       </c>
       <c r="C95">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B96" t="s">
         <v>280</v>
       </c>
       <c r="C96">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="C97">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>181</v>
       </c>
       <c r="B98" t="s">
-        <v>297</v>
+        <v>280</v>
       </c>
       <c r="C98">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>98</v>
+        <v>133</v>
       </c>
       <c r="B99" t="s">
-        <v>278</v>
+        <v>321</v>
       </c>
       <c r="C99">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>99</v>
+        <v>191</v>
       </c>
       <c r="B100" t="s">
-        <v>300</v>
+        <v>321</v>
       </c>
       <c r="C100">
-        <v>0</v>
+        <v>9</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>100</v>
+        <v>240</v>
       </c>
       <c r="B101" t="s">
-        <v>293</v>
-      </c>
-      <c r="C101" t="s">
-        <v>346</v>
+        <v>321</v>
+      </c>
+      <c r="C101">
+        <v>8</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>101</v>
+        <v>250</v>
       </c>
       <c r="B102" t="s">
-        <v>275</v>
+        <v>321</v>
       </c>
       <c r="C102">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>102</v>
+        <v>253</v>
       </c>
       <c r="B103" t="s">
-        <v>297</v>
-      </c>
-      <c r="C103" t="s">
-        <v>346</v>
+        <v>321</v>
+      </c>
+      <c r="C103">
+        <v>5</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="B104" t="s">
-        <v>275</v>
+        <v>336</v>
       </c>
       <c r="C104">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>104</v>
+        <v>232</v>
       </c>
       <c r="B105" t="s">
-        <v>297</v>
+        <v>350</v>
       </c>
       <c r="C105">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>105</v>
+        <v>244</v>
       </c>
       <c r="B106" t="s">
-        <v>313</v>
+        <v>350</v>
       </c>
       <c r="C106">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>106</v>
+        <v>268</v>
       </c>
       <c r="B107" t="s">
-        <v>314</v>
+        <v>350</v>
       </c>
       <c r="C107">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>65</v>
       </c>
       <c r="B108" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="C108">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>108</v>
+        <v>143</v>
       </c>
       <c r="B109" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="C109">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>109</v>
+        <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C110">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="B111" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C111">
         <v>3</v>
@@ -2750,98 +2757,98 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="B112" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="C112">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B113" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="C113">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>113</v>
+        <v>219</v>
       </c>
       <c r="B114" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="C114">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>114</v>
+        <v>261</v>
       </c>
       <c r="B115" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C115">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>115</v>
+        <v>60</v>
       </c>
       <c r="B116" t="s">
-        <v>275</v>
+        <v>304</v>
       </c>
       <c r="C116">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>116</v>
+        <v>64</v>
       </c>
       <c r="B117" t="s">
-        <v>280</v>
+        <v>304</v>
       </c>
       <c r="C117">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>117</v>
+        <v>3</v>
       </c>
       <c r="B118" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C118">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>35</v>
       </c>
       <c r="B119" t="s">
         <v>278</v>
       </c>
       <c r="C119">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>119</v>
+        <v>49</v>
       </c>
       <c r="B120" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="C120">
         <v>3</v>
@@ -2849,13 +2856,13 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="B121" t="s">
-        <v>364</v>
+        <v>278</v>
       </c>
       <c r="C121">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
@@ -2863,7 +2870,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="C122">
         <v>2</v>
@@ -2871,65 +2878,65 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B123" t="s">
         <v>278</v>
       </c>
       <c r="C123">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="B124" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C124">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>124</v>
+        <v>175</v>
       </c>
       <c r="B125" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C125">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="B126" t="s">
         <v>278</v>
       </c>
       <c r="C126">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>126</v>
+        <v>186</v>
       </c>
       <c r="B127" t="s">
-        <v>365</v>
+        <v>278</v>
       </c>
       <c r="C127">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>127</v>
+        <v>196</v>
       </c>
       <c r="B128" t="s">
-        <v>309</v>
+        <v>278</v>
       </c>
       <c r="C128">
         <v>7</v>
@@ -2937,76 +2944,76 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>128</v>
+        <v>213</v>
       </c>
       <c r="B129" t="s">
-        <v>317</v>
+        <v>278</v>
       </c>
       <c r="C129">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="B130" t="s">
-        <v>280</v>
+        <v>338</v>
       </c>
       <c r="C130">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="B131" t="s">
-        <v>318</v>
+        <v>329</v>
       </c>
       <c r="C131">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>131</v>
+        <v>18</v>
       </c>
       <c r="B132" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="C132">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>132</v>
+        <v>184</v>
       </c>
       <c r="B133" t="s">
-        <v>319</v>
+        <v>298</v>
       </c>
       <c r="C133">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>133</v>
+        <v>16</v>
       </c>
       <c r="B134" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="C134">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>134</v>
+        <v>254</v>
       </c>
       <c r="B135" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C135">
         <v>5</v>
@@ -3014,145 +3021,145 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>135</v>
+        <v>94</v>
       </c>
       <c r="B136" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C136">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="B137" t="s">
-        <v>275</v>
+        <v>312</v>
       </c>
       <c r="C137">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>137</v>
+        <v>105</v>
       </c>
       <c r="B138" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C138">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>138</v>
+        <v>199</v>
       </c>
       <c r="B139" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C139">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>139</v>
+        <v>38</v>
       </c>
       <c r="B140" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="C140">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>140</v>
+        <v>258</v>
       </c>
       <c r="B141" t="s">
-        <v>322</v>
+        <v>355</v>
       </c>
       <c r="C141">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>141</v>
+        <v>26</v>
       </c>
       <c r="B142" t="s">
-        <v>275</v>
+        <v>294</v>
       </c>
       <c r="C142">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="B143" t="s">
-        <v>323</v>
+        <v>294</v>
       </c>
       <c r="C143">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>143</v>
+        <v>96</v>
       </c>
       <c r="B144" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="C144">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>144</v>
+        <v>156</v>
       </c>
       <c r="B145" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
       <c r="C145">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>145</v>
+        <v>236</v>
       </c>
       <c r="B146" t="s">
-        <v>325</v>
+        <v>313</v>
       </c>
       <c r="C146">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
       <c r="B147" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="C147">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="B148" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C148">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
@@ -3160,7 +3167,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -3168,43 +3175,43 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="B150" t="s">
-        <v>275</v>
+        <v>323</v>
       </c>
       <c r="C150">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="B151" t="s">
-        <v>275</v>
+        <v>337</v>
       </c>
       <c r="C151">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>151</v>
+        <v>1</v>
       </c>
       <c r="B152" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C152">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>327</v>
+        <v>276</v>
       </c>
       <c r="C153">
         <v>4</v>
@@ -3212,65 +3219,65 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>153</v>
+        <v>19</v>
       </c>
       <c r="B154" t="s">
-        <v>328</v>
+        <v>276</v>
       </c>
       <c r="C154">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>154</v>
+        <v>22</v>
       </c>
       <c r="B155" t="s">
-        <v>329</v>
+        <v>276</v>
       </c>
       <c r="C155">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>155</v>
+        <v>42</v>
       </c>
       <c r="B156" t="s">
-        <v>366</v>
+        <v>276</v>
       </c>
       <c r="C156">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>362</v>
+        <v>55</v>
       </c>
       <c r="B157" t="s">
-        <v>312</v>
+        <v>276</v>
       </c>
       <c r="C157">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>69</v>
       </c>
       <c r="B158" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C158">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>79</v>
       </c>
       <c r="B159" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="C159">
         <v>4</v>
@@ -3278,230 +3285,230 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>86</v>
       </c>
       <c r="B160" t="s">
-        <v>322</v>
+        <v>276</v>
       </c>
       <c r="C160">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>87</v>
       </c>
       <c r="B161" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
       <c r="C161">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>89</v>
       </c>
       <c r="B162" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="C162">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>101</v>
       </c>
       <c r="B163" t="s">
-        <v>330</v>
+        <v>276</v>
       </c>
       <c r="C163">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>103</v>
       </c>
       <c r="B164" t="s">
-        <v>367</v>
+        <v>276</v>
       </c>
       <c r="C164">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>109</v>
       </c>
       <c r="B165" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C165">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>110</v>
       </c>
       <c r="B166" t="s">
-        <v>331</v>
-      </c>
-      <c r="C166" t="s">
-        <v>346</v>
+        <v>276</v>
+      </c>
+      <c r="C166">
+        <v>3</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>113</v>
       </c>
       <c r="B167" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="C167">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>115</v>
       </c>
       <c r="B168" t="s">
-        <v>329</v>
+        <v>276</v>
       </c>
       <c r="C168">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>119</v>
       </c>
       <c r="B169" t="s">
-        <v>368</v>
+        <v>276</v>
       </c>
       <c r="C169">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>136</v>
       </c>
       <c r="B170" t="s">
-        <v>332</v>
+        <v>276</v>
       </c>
       <c r="C170">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="B171" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="C171">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>149</v>
       </c>
       <c r="B172" t="s">
-        <v>333</v>
+        <v>276</v>
       </c>
       <c r="C172">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>150</v>
       </c>
       <c r="B173" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="C173">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
       <c r="B174" t="s">
-        <v>369</v>
+        <v>276</v>
       </c>
       <c r="C174">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B175" t="s">
-        <v>334</v>
+        <v>276</v>
       </c>
       <c r="C175">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="B176" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C176">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="B177" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C177">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c r="B178" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C178">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>176</v>
+        <v>200</v>
       </c>
       <c r="B179" t="s">
-        <v>327</v>
+        <v>276</v>
       </c>
       <c r="C179">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="B180" t="s">
-        <v>335</v>
+        <v>276</v>
       </c>
       <c r="C180">
         <v>1</v>
@@ -3509,219 +3516,219 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>178</v>
+        <v>211</v>
       </c>
       <c r="B181" t="s">
-        <v>297</v>
+        <v>276</v>
       </c>
       <c r="C181">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>179</v>
+        <v>216</v>
       </c>
       <c r="B182" t="s">
-        <v>336</v>
+        <v>276</v>
       </c>
       <c r="C182">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>217</v>
       </c>
       <c r="B183" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C183">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>181</v>
+        <v>228</v>
       </c>
       <c r="B184" t="s">
-        <v>300</v>
+        <v>276</v>
       </c>
       <c r="C184">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>182</v>
+        <v>230</v>
       </c>
       <c r="B185" t="s">
-        <v>337</v>
+        <v>276</v>
       </c>
       <c r="C185">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>183</v>
+        <v>245</v>
       </c>
       <c r="B186" t="s">
-        <v>370</v>
+        <v>276</v>
       </c>
       <c r="C186">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>184</v>
+        <v>260</v>
       </c>
       <c r="B187" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C187">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>185</v>
+        <v>269</v>
       </c>
       <c r="B188" t="s">
-        <v>369</v>
+        <v>276</v>
       </c>
       <c r="C188">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>186</v>
+        <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>275</v>
+        <v>309</v>
       </c>
       <c r="C189">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>187</v>
+        <v>160</v>
       </c>
       <c r="B190" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="C190">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>286</v>
-      </c>
-      <c r="C191" t="s">
-        <v>346</v>
+        <v>309</v>
+      </c>
+      <c r="C191">
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
       <c r="B192" t="s">
-        <v>308</v>
-      </c>
-      <c r="C192" t="s">
-        <v>346</v>
+        <v>309</v>
+      </c>
+      <c r="C192">
+        <v>7</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>190</v>
+        <v>241</v>
       </c>
       <c r="B193" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="C193">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>191</v>
+        <v>203</v>
       </c>
       <c r="B194" t="s">
-        <v>297</v>
+        <v>341</v>
       </c>
       <c r="C194">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>192</v>
+        <v>11</v>
       </c>
       <c r="B195" t="s">
-        <v>338</v>
+        <v>284</v>
       </c>
       <c r="C195">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>193</v>
+        <v>251</v>
       </c>
       <c r="B196" t="s">
-        <v>371</v>
+        <v>354</v>
       </c>
       <c r="C196">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>194</v>
+        <v>130</v>
       </c>
       <c r="B197" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C197">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>195</v>
+        <v>154</v>
       </c>
       <c r="B198" t="s">
-        <v>369</v>
+        <v>330</v>
       </c>
       <c r="C198">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>196</v>
+        <v>167</v>
       </c>
       <c r="B199" t="s">
-        <v>275</v>
+        <v>330</v>
       </c>
       <c r="C199">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>197</v>
+        <v>239</v>
       </c>
       <c r="B200" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C200">
         <v>3</v>
@@ -3729,65 +3736,65 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>198</v>
+        <v>259</v>
       </c>
       <c r="B201" t="s">
-        <v>313</v>
+        <v>330</v>
       </c>
       <c r="C201">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>199</v>
+        <v>169</v>
       </c>
       <c r="B202" t="s">
-        <v>275</v>
+        <v>333</v>
       </c>
       <c r="C202">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>200</v>
+        <v>274</v>
       </c>
       <c r="B203" t="s">
-        <v>291</v>
+        <v>333</v>
       </c>
       <c r="C203">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>201</v>
+        <v>162</v>
       </c>
       <c r="B204" t="s">
-        <v>275</v>
+        <v>331</v>
       </c>
       <c r="C204">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>202</v>
+        <v>68</v>
       </c>
       <c r="B205" t="s">
-        <v>340</v>
+        <v>306</v>
       </c>
       <c r="C205">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
       <c r="B206" t="s">
-        <v>286</v>
+        <v>317</v>
       </c>
       <c r="C206">
         <v>0</v>
@@ -3795,21 +3802,21 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>204</v>
+        <v>108</v>
       </c>
       <c r="B207" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="C207">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>205</v>
+        <v>138</v>
       </c>
       <c r="B208" t="s">
-        <v>341</v>
+        <v>317</v>
       </c>
       <c r="C208">
         <v>0</v>
@@ -3817,54 +3824,54 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>206</v>
+        <v>146</v>
       </c>
       <c r="B209" t="s">
-        <v>342</v>
+        <v>317</v>
       </c>
       <c r="C209">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>207</v>
+        <v>168</v>
       </c>
       <c r="B210" t="s">
-        <v>371</v>
+        <v>317</v>
       </c>
       <c r="C210">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>208</v>
+        <v>31</v>
       </c>
       <c r="B211" t="s">
-        <v>343</v>
-      </c>
-      <c r="C211" t="s">
-        <v>346</v>
+        <v>296</v>
+      </c>
+      <c r="C211">
+        <v>1</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>209</v>
+        <v>32</v>
       </c>
       <c r="B212" t="s">
-        <v>286</v>
+        <v>297</v>
       </c>
       <c r="C212">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>210</v>
+        <v>36</v>
       </c>
       <c r="B213" t="s">
-        <v>275</v>
+        <v>297</v>
       </c>
       <c r="C213">
         <v>4</v>
@@ -3872,109 +3879,109 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>211</v>
+        <v>54</v>
       </c>
       <c r="B214" t="s">
-        <v>372</v>
+        <v>297</v>
       </c>
       <c r="C214">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="B215" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="C215">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>213</v>
+        <v>266</v>
       </c>
       <c r="B216" t="s">
-        <v>310</v>
-      </c>
-      <c r="C216" t="s">
-        <v>346</v>
+        <v>358</v>
+      </c>
+      <c r="C216">
+        <v>2</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="B217" t="s">
-        <v>286</v>
+        <v>347</v>
       </c>
       <c r="C217">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>215</v>
+        <v>134</v>
       </c>
       <c r="B218" t="s">
-        <v>275</v>
-      </c>
-      <c r="C218" t="s">
-        <v>346</v>
+        <v>322</v>
+      </c>
+      <c r="C218">
+        <v>5</v>
       </c>
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="B219" t="s">
-        <v>275</v>
+        <v>346</v>
       </c>
       <c r="C219">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>217</v>
+        <v>242</v>
       </c>
       <c r="B220" t="s">
-        <v>302</v>
-      </c>
-      <c r="C220" t="s">
         <v>346</v>
+      </c>
+      <c r="C220">
+        <v>3</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="B221" t="s">
-        <v>280</v>
+        <v>326</v>
       </c>
       <c r="C221">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B222" t="s">
-        <v>281</v>
+        <v>326</v>
       </c>
       <c r="C222">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>220</v>
+        <v>15</v>
       </c>
       <c r="B223" t="s">
-        <v>344</v>
+        <v>287</v>
       </c>
       <c r="C223">
         <v>3</v>
@@ -3982,43 +3989,43 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>221</v>
+        <v>37</v>
       </c>
       <c r="B224" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
       <c r="C224">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>222</v>
+        <v>111</v>
       </c>
       <c r="B225" t="s">
-        <v>309</v>
+        <v>287</v>
       </c>
       <c r="C225">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>223</v>
+        <v>123</v>
       </c>
       <c r="B226" t="s">
-        <v>308</v>
+        <v>287</v>
       </c>
       <c r="C226">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>224</v>
+        <v>173</v>
       </c>
       <c r="B227" t="s">
-        <v>345</v>
+        <v>287</v>
       </c>
       <c r="C227">
         <v>2</v>
@@ -4026,43 +4033,43 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>225</v>
+        <v>176</v>
       </c>
       <c r="B228" t="s">
-        <v>346</v>
-      </c>
-      <c r="C228" t="s">
-        <v>346</v>
+        <v>287</v>
+      </c>
+      <c r="C228">
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="B229" t="s">
-        <v>347</v>
+        <v>287</v>
       </c>
       <c r="C229">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="B230" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="C230">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="B231" t="s">
-        <v>348</v>
+        <v>287</v>
       </c>
       <c r="C231">
         <v>5</v>
@@ -4070,98 +4077,98 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B232" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="C232">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>230</v>
+        <v>246</v>
       </c>
       <c r="B233" t="s">
-        <v>373</v>
-      </c>
-      <c r="C233" t="s">
-        <v>346</v>
+        <v>287</v>
+      </c>
+      <c r="C233">
+        <v>1</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>231</v>
+        <v>263</v>
       </c>
       <c r="B234" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
       <c r="C234">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>232</v>
+        <v>165</v>
       </c>
       <c r="B235" t="s">
-        <v>350</v>
+        <v>332</v>
       </c>
       <c r="C235">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>233</v>
+        <v>247</v>
       </c>
       <c r="B236" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="C236">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="B237" t="s">
-        <v>281</v>
+        <v>342</v>
       </c>
       <c r="C237">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>235</v>
+        <v>72</v>
       </c>
       <c r="B238" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C238">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>236</v>
+        <v>17</v>
       </c>
       <c r="B239" t="s">
-        <v>350</v>
+        <v>289</v>
       </c>
       <c r="C239">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>237</v>
+        <v>48</v>
       </c>
       <c r="B240" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="C240">
         <v>4</v>
@@ -4169,98 +4176,98 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>238</v>
+        <v>66</v>
       </c>
       <c r="B241" t="s">
-        <v>329</v>
+        <v>289</v>
       </c>
       <c r="C241">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>239</v>
+        <v>71</v>
       </c>
       <c r="B242" t="s">
-        <v>320</v>
+        <v>289</v>
       </c>
       <c r="C242">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>240</v>
+        <v>161</v>
       </c>
       <c r="B243" t="s">
-        <v>308</v>
+        <v>289</v>
       </c>
       <c r="C243">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B244" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C244">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>242</v>
+        <v>58</v>
       </c>
       <c r="B245" t="s">
-        <v>352</v>
+        <v>303</v>
       </c>
       <c r="C245">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>243</v>
+        <v>218</v>
       </c>
       <c r="B246" t="s">
-        <v>349</v>
+        <v>303</v>
       </c>
       <c r="C246">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>244</v>
+        <v>267</v>
       </c>
       <c r="B247" t="s">
-        <v>275</v>
+        <v>359</v>
       </c>
       <c r="C247">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>245</v>
+        <v>20</v>
       </c>
       <c r="B248" t="s">
-        <v>286</v>
+        <v>291</v>
       </c>
       <c r="C248">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>246</v>
+        <v>171</v>
       </c>
       <c r="B249" t="s">
-        <v>374</v>
+        <v>334</v>
       </c>
       <c r="C249">
         <v>5</v>
@@ -4268,197 +4275,197 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>247</v>
+        <v>34</v>
       </c>
       <c r="B250" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C250">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>248</v>
+        <v>41</v>
       </c>
       <c r="B251" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="C251">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>249</v>
+        <v>50</v>
       </c>
       <c r="B252" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="C252">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>250</v>
+        <v>51</v>
       </c>
       <c r="B253" t="s">
-        <v>353</v>
+        <v>298</v>
       </c>
       <c r="C253">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>251</v>
+        <v>59</v>
       </c>
       <c r="B254" t="s">
-        <v>285</v>
-      </c>
-      <c r="C254" t="s">
-        <v>346</v>
+        <v>298</v>
+      </c>
+      <c r="C254">
+        <v>7</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>252</v>
+        <v>75</v>
       </c>
       <c r="B255" t="s">
-        <v>320</v>
+        <v>298</v>
       </c>
       <c r="C255">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>253</v>
+        <v>81</v>
       </c>
       <c r="B256" t="s">
-        <v>375</v>
+        <v>298</v>
       </c>
       <c r="C256">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>254</v>
+        <v>82</v>
       </c>
       <c r="B257" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C257">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>255</v>
+        <v>85</v>
       </c>
       <c r="B258" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C258">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>256</v>
+        <v>93</v>
       </c>
       <c r="B259" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C259">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>257</v>
+        <v>97</v>
       </c>
       <c r="B260" t="s">
-        <v>354</v>
+        <v>298</v>
       </c>
       <c r="C260">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>258</v>
+        <v>102</v>
       </c>
       <c r="B261" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="C261">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>259</v>
+        <v>104</v>
       </c>
       <c r="B262" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="C262">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>260</v>
+        <v>166</v>
       </c>
       <c r="B263" t="s">
-        <v>280</v>
+        <v>298</v>
       </c>
       <c r="C263">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>261</v>
+        <v>170</v>
       </c>
       <c r="B264" t="s">
-        <v>355</v>
+        <v>298</v>
       </c>
       <c r="C264">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>262</v>
+        <v>179</v>
       </c>
       <c r="B265" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C265">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>263</v>
+        <v>192</v>
       </c>
       <c r="B266" t="s">
-        <v>356</v>
+        <v>298</v>
       </c>
       <c r="C266">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C267">
         <v>4</v>
@@ -4466,21 +4473,21 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>265</v>
+        <v>271</v>
       </c>
       <c r="B268" t="s">
-        <v>357</v>
+        <v>298</v>
       </c>
       <c r="C268">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>266</v>
+        <v>194</v>
       </c>
       <c r="B269" t="s">
-        <v>358</v>
+        <v>298</v>
       </c>
       <c r="C269">
         <v>3</v>
@@ -4488,82 +4495,85 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>267</v>
+        <v>208</v>
       </c>
       <c r="B270" t="s">
-        <v>349</v>
+        <v>298</v>
       </c>
       <c r="C270">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>268</v>
+        <v>212</v>
       </c>
       <c r="B271" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="C271">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>269</v>
+        <v>46</v>
       </c>
       <c r="B272" t="s">
         <v>300</v>
       </c>
       <c r="C272">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>270</v>
+        <v>73</v>
       </c>
       <c r="B273" t="s">
-        <v>297</v>
+        <v>308</v>
       </c>
       <c r="C273">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>271</v>
+        <v>152</v>
       </c>
       <c r="B274" t="s">
-        <v>359</v>
+        <v>328</v>
       </c>
       <c r="C274">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>272</v>
+        <v>177</v>
       </c>
       <c r="B275" t="s">
-        <v>360</v>
+        <v>328</v>
       </c>
       <c r="C275">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>273</v>
+        <v>243</v>
       </c>
       <c r="B276" t="s">
-        <v>332</v>
+        <v>353</v>
       </c>
       <c r="C276">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
replaced multiple occupations with 'Multiple Occupations'
</commit_message>
<xml_diff>
--- a/fertility_occupation.xlsx
+++ b/fertility_occupation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="558" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="559" uniqueCount="352">
   <si>
     <t>MP</t>
   </si>
@@ -857,9 +857,6 @@
     <t>Lawyer</t>
   </si>
   <si>
-    <t>Banker/Lecturer</t>
-  </si>
-  <si>
     <t>Farmer</t>
   </si>
   <si>
@@ -932,9 +929,6 @@
     <t>Accountant</t>
   </si>
   <si>
-    <t>Consultant, Health</t>
-  </si>
-  <si>
     <t>Social Worker</t>
   </si>
   <si>
@@ -992,12 +986,6 @@
     <t>Educationist</t>
   </si>
   <si>
-    <t>Network engineer/ Bussiness person</t>
-  </si>
-  <si>
-    <t>Journalist/Advertiser</t>
-  </si>
-  <si>
     <t>Business person</t>
   </si>
   <si>
@@ -1013,51 +1001,24 @@
     <t>Veterinary Surgeon</t>
   </si>
   <si>
-    <t>Fashion designer/Politician</t>
-  </si>
-  <si>
-    <t>Manager/Administrator</t>
-  </si>
-  <si>
     <t>Managing Director</t>
   </si>
   <si>
     <t>Project Manager</t>
   </si>
   <si>
-    <t>Manager/Administrator/HR Practitioner</t>
-  </si>
-  <si>
     <t>Tax Administrator</t>
   </si>
   <si>
     <t>Administrator</t>
   </si>
   <si>
-    <t>Educationist/Development Planning</t>
-  </si>
-  <si>
     <t>Jourrnalist</t>
   </si>
   <si>
-    <t>Farmer/Social Worker</t>
-  </si>
-  <si>
-    <t>Economist/Banker/Insurer</t>
-  </si>
-  <si>
-    <t>Education / Agriculture</t>
-  </si>
-  <si>
-    <t>Lecturer/Development Consultant</t>
-  </si>
-  <si>
     <t>Psychologist</t>
   </si>
   <si>
-    <t xml:space="preserve"> PR/Journalist/Advertiser/Marketer</t>
-  </si>
-  <si>
     <t>Retired Deputy Director of Ghana Prisons Service</t>
   </si>
   <si>
@@ -1073,27 +1034,15 @@
     <t>DCE</t>
   </si>
   <si>
-    <t>Economist/Banker</t>
-  </si>
-  <si>
-    <t>Educationist/Teacher</t>
-  </si>
-  <si>
     <t>Chartered Accountant</t>
   </si>
   <si>
-    <t>Accounting,Economics, Commerce</t>
-  </si>
-  <si>
     <t>Youth in Dev. &amp; Work</t>
   </si>
   <si>
     <t>Local Government Practitioner</t>
   </si>
   <si>
-    <t>Investment Manager, COCOBOD</t>
-  </si>
-  <si>
     <t>Army Officer</t>
   </si>
   <si>
@@ -1106,12 +1055,6 @@
     <t>Storekeeper</t>
   </si>
   <si>
-    <t>Biochemist/Hotelier</t>
-  </si>
-  <si>
-    <t>Medical Doctor/Nurse/Health Worker</t>
-  </si>
-  <si>
     <t>Kids</t>
   </si>
   <si>
@@ -1131,6 +1074,12 @@
   </si>
   <si>
     <t>I also replaced N/A with 0 for MPs who had N/A for number of kids</t>
+  </si>
+  <si>
+    <t>I also replaced all occuptions of MPs who indicated they do multiple jobs with "Multiple Occupations"</t>
+  </si>
+  <si>
+    <t>Multiple Occupations</t>
   </si>
 </sst>
 </file>
@@ -1509,7 +1458,7 @@
   <dimension ref="A1:H276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,7 +1475,7 @@
         <v>275</v>
       </c>
       <c r="C1" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1534,7 +1483,7 @@
         <v>207</v>
       </c>
       <c r="B2" t="s">
-        <v>343</v>
+        <v>351</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -1546,16 +1495,16 @@
         <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3">
         <v>7</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="H3" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -1563,16 +1512,16 @@
         <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="G4" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1580,13 +1529,13 @@
         <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C5">
         <v>6</v>
       </c>
       <c r="G5" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1594,10 +1543,13 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C6">
         <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1605,7 +1557,7 @@
         <v>77</v>
       </c>
       <c r="B7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1616,7 +1568,7 @@
         <v>80</v>
       </c>
       <c r="B8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C8">
         <v>2</v>
@@ -1627,7 +1579,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1638,7 +1590,7 @@
         <v>172</v>
       </c>
       <c r="B10" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -1649,7 +1601,7 @@
         <v>182</v>
       </c>
       <c r="B11" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -1660,7 +1612,7 @@
         <v>188</v>
       </c>
       <c r="B12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1671,7 +1623,7 @@
         <v>205</v>
       </c>
       <c r="B13" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C13">
         <v>4</v>
@@ -1682,7 +1634,7 @@
         <v>255</v>
       </c>
       <c r="B14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -1693,7 +1645,7 @@
         <v>256</v>
       </c>
       <c r="B15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -1704,7 +1656,7 @@
         <v>270</v>
       </c>
       <c r="B16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -1715,7 +1667,7 @@
         <v>238</v>
       </c>
       <c r="B17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1726,7 +1678,7 @@
         <v>174</v>
       </c>
       <c r="B18" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C18">
         <v>0</v>
@@ -1737,7 +1689,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -1748,7 +1700,7 @@
         <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C20">
         <v>3</v>
@@ -1759,7 +1711,7 @@
         <v>147</v>
       </c>
       <c r="B21" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="C21">
         <v>3</v>
@@ -1770,7 +1722,7 @@
         <v>90</v>
       </c>
       <c r="B22" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C22">
         <v>4</v>
@@ -1781,7 +1733,7 @@
         <v>127</v>
       </c>
       <c r="B23" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C23">
         <v>7</v>
@@ -1792,7 +1744,7 @@
         <v>223</v>
       </c>
       <c r="B24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C24">
         <v>3</v>
@@ -1803,7 +1755,7 @@
         <v>234</v>
       </c>
       <c r="B25" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C25">
         <v>4</v>
@@ -1814,7 +1766,7 @@
         <v>262</v>
       </c>
       <c r="B26" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="C26">
         <v>3</v>
@@ -1825,7 +1777,7 @@
         <v>91</v>
       </c>
       <c r="B27" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C27">
         <v>1</v>
@@ -1836,7 +1788,7 @@
         <v>214</v>
       </c>
       <c r="B28" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="C28">
         <v>0</v>
@@ -1847,7 +1799,7 @@
         <v>13</v>
       </c>
       <c r="B29" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C29">
         <v>3</v>
@@ -1858,7 +1810,7 @@
         <v>40</v>
       </c>
       <c r="B30" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -1869,7 +1821,7 @@
         <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C31">
         <v>5</v>
@@ -1880,7 +1832,7 @@
         <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C32">
         <v>3</v>
@@ -1891,7 +1843,7 @@
         <v>88</v>
       </c>
       <c r="B33" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C33">
         <v>5</v>
@@ -1902,7 +1854,7 @@
         <v>114</v>
       </c>
       <c r="B34" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C34">
         <v>2</v>
@@ -1913,7 +1865,7 @@
         <v>117</v>
       </c>
       <c r="B35" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C35">
         <v>7</v>
@@ -1924,7 +1876,7 @@
         <v>158</v>
       </c>
       <c r="B36" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -1935,7 +1887,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>277</v>
+        <v>351</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -1946,7 +1898,7 @@
         <v>120</v>
       </c>
       <c r="B38" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="C38">
         <v>3</v>
@@ -1957,7 +1909,7 @@
         <v>272</v>
       </c>
       <c r="B39" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -1968,7 +1920,7 @@
         <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C40">
         <v>6</v>
@@ -1979,7 +1931,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C41">
         <v>3</v>
@@ -1990,7 +1942,7 @@
         <v>24</v>
       </c>
       <c r="B42" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C42">
         <v>2</v>
@@ -2001,7 +1953,7 @@
         <v>28</v>
       </c>
       <c r="B43" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C43">
         <v>10</v>
@@ -2012,7 +1964,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C44">
         <v>6</v>
@@ -2023,7 +1975,7 @@
         <v>53</v>
       </c>
       <c r="B45" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C45">
         <v>1</v>
@@ -2034,7 +1986,7 @@
         <v>78</v>
       </c>
       <c r="B46" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C46">
         <v>4</v>
@@ -2045,7 +1997,7 @@
         <v>98</v>
       </c>
       <c r="B47" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C47">
         <v>3</v>
@@ -2056,7 +2008,7 @@
         <v>118</v>
       </c>
       <c r="B48" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -2067,7 +2019,7 @@
         <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C49">
         <v>0</v>
@@ -2078,7 +2030,7 @@
         <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C50">
         <v>3</v>
@@ -2089,7 +2041,7 @@
         <v>131</v>
       </c>
       <c r="B51" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C51">
         <v>5</v>
@@ -2100,7 +2052,7 @@
         <v>137</v>
       </c>
       <c r="B52" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C52">
         <v>6</v>
@@ -2111,7 +2063,7 @@
         <v>139</v>
       </c>
       <c r="B53" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -2122,7 +2074,7 @@
         <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C54">
         <v>4</v>
@@ -2133,7 +2085,7 @@
         <v>195</v>
       </c>
       <c r="B55" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C55">
         <v>3</v>
@@ -2144,7 +2096,7 @@
         <v>248</v>
       </c>
       <c r="B56" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C56">
         <v>3</v>
@@ -2155,7 +2107,7 @@
         <v>257</v>
       </c>
       <c r="B57" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C57">
         <v>5</v>
@@ -2166,7 +2118,7 @@
         <v>107</v>
       </c>
       <c r="B58" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="C58">
         <v>4</v>
@@ -2177,7 +2129,7 @@
         <v>233</v>
       </c>
       <c r="B59" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C59">
         <v>7</v>
@@ -2188,7 +2140,7 @@
         <v>237</v>
       </c>
       <c r="B60" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C60">
         <v>2</v>
@@ -2199,7 +2151,7 @@
         <v>221</v>
       </c>
       <c r="B61" t="s">
-        <v>345</v>
+        <v>332</v>
       </c>
       <c r="C61">
         <v>3</v>
@@ -2210,7 +2162,7 @@
         <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C62">
         <v>3</v>
@@ -2221,7 +2173,7 @@
         <v>30</v>
       </c>
       <c r="B63" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C63">
         <v>3</v>
@@ -2232,7 +2184,7 @@
         <v>201</v>
       </c>
       <c r="B64" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C64">
         <v>6</v>
@@ -2243,7 +2195,7 @@
         <v>264</v>
       </c>
       <c r="B65" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
       <c r="C65">
         <v>3</v>
@@ -2254,7 +2206,7 @@
         <v>29</v>
       </c>
       <c r="B66" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C66">
         <v>6</v>
@@ -2265,7 +2217,7 @@
         <v>128</v>
       </c>
       <c r="B67" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="C67">
         <v>3</v>
@@ -2276,7 +2228,7 @@
         <v>57</v>
       </c>
       <c r="B68" t="s">
-        <v>302</v>
+        <v>351</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -2287,7 +2239,7 @@
         <v>106</v>
       </c>
       <c r="B69" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C69">
         <v>3</v>
@@ -2298,7 +2250,7 @@
         <v>227</v>
       </c>
       <c r="B70" t="s">
-        <v>348</v>
+        <v>335</v>
       </c>
       <c r="C70">
         <v>2</v>
@@ -2309,7 +2261,7 @@
         <v>144</v>
       </c>
       <c r="B71" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="C71">
         <v>3</v>
@@ -2320,7 +2272,7 @@
         <v>8</v>
       </c>
       <c r="B72" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C72">
         <v>4</v>
@@ -2331,7 +2283,7 @@
         <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C73">
         <v>4</v>
@@ -2342,7 +2294,7 @@
         <v>33</v>
       </c>
       <c r="B74" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C74">
         <v>5</v>
@@ -2353,7 +2305,7 @@
         <v>220</v>
       </c>
       <c r="B75" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C75">
         <v>6</v>
@@ -2364,7 +2316,7 @@
         <v>235</v>
       </c>
       <c r="B76" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C76">
         <v>3</v>
@@ -2375,7 +2327,7 @@
         <v>132</v>
       </c>
       <c r="B77" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C77">
         <v>4</v>
@@ -2386,7 +2338,7 @@
         <v>14</v>
       </c>
       <c r="B78" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C78">
         <v>5</v>
@@ -2397,7 +2349,7 @@
         <v>21</v>
       </c>
       <c r="B79" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C79">
         <v>5</v>
@@ -2408,7 +2360,7 @@
         <v>39</v>
       </c>
       <c r="B80" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C80">
         <v>3</v>
@@ -2419,7 +2371,7 @@
         <v>44</v>
       </c>
       <c r="B81" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C81">
         <v>3</v>
@@ -2430,7 +2382,7 @@
         <v>47</v>
       </c>
       <c r="B82" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C82">
         <v>5</v>
@@ -2441,7 +2393,7 @@
         <v>76</v>
       </c>
       <c r="B83" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C83">
         <v>7</v>
@@ -2452,7 +2404,7 @@
         <v>124</v>
       </c>
       <c r="B84" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C84">
         <v>3</v>
@@ -2463,7 +2415,7 @@
         <v>249</v>
       </c>
       <c r="B85" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C85">
         <v>4</v>
@@ -2474,7 +2426,7 @@
         <v>252</v>
       </c>
       <c r="B86" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C86">
         <v>0</v>
@@ -2485,7 +2437,7 @@
         <v>229</v>
       </c>
       <c r="B87" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C87">
         <v>5</v>
@@ -2496,7 +2448,7 @@
         <v>193</v>
       </c>
       <c r="B88" t="s">
-        <v>339</v>
+        <v>351</v>
       </c>
       <c r="C88">
         <v>7</v>
@@ -2507,7 +2459,7 @@
         <v>198</v>
       </c>
       <c r="B89" t="s">
-        <v>340</v>
+        <v>351</v>
       </c>
       <c r="C89">
         <v>3</v>
@@ -2518,7 +2470,7 @@
         <v>5</v>
       </c>
       <c r="B90" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C90">
         <v>3</v>
@@ -2529,7 +2481,7 @@
         <v>7</v>
       </c>
       <c r="B91" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -2540,7 +2492,7 @@
         <v>27</v>
       </c>
       <c r="B92" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C92">
         <v>2</v>
@@ -2551,7 +2503,7 @@
         <v>52</v>
       </c>
       <c r="B93" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C93">
         <v>5</v>
@@ -2562,7 +2514,7 @@
         <v>61</v>
       </c>
       <c r="B94" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C94">
         <v>6</v>
@@ -2573,7 +2525,7 @@
         <v>67</v>
       </c>
       <c r="B95" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C95">
         <v>4</v>
@@ -2584,7 +2536,7 @@
         <v>92</v>
       </c>
       <c r="B96" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C96">
         <v>4</v>
@@ -2595,7 +2547,7 @@
         <v>112</v>
       </c>
       <c r="B97" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C97">
         <v>3</v>
@@ -2606,7 +2558,7 @@
         <v>181</v>
       </c>
       <c r="B98" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C98">
         <v>6</v>
@@ -2617,7 +2569,7 @@
         <v>133</v>
       </c>
       <c r="B99" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C99">
         <v>1</v>
@@ -2628,7 +2580,7 @@
         <v>191</v>
       </c>
       <c r="B100" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C100">
         <v>9</v>
@@ -2639,7 +2591,7 @@
         <v>240</v>
       </c>
       <c r="B101" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C101">
         <v>8</v>
@@ -2650,7 +2602,7 @@
         <v>250</v>
       </c>
       <c r="B102" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C102">
         <v>0</v>
@@ -2661,7 +2613,7 @@
         <v>253</v>
       </c>
       <c r="B103" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C103">
         <v>5</v>
@@ -2672,7 +2624,7 @@
         <v>178</v>
       </c>
       <c r="B104" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -2683,7 +2635,7 @@
         <v>232</v>
       </c>
       <c r="B105" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C105">
         <v>3</v>
@@ -2694,7 +2646,7 @@
         <v>244</v>
       </c>
       <c r="B106" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C106">
         <v>5</v>
@@ -2705,7 +2657,7 @@
         <v>268</v>
       </c>
       <c r="B107" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C107">
         <v>5</v>
@@ -2716,7 +2668,7 @@
         <v>65</v>
       </c>
       <c r="B108" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C108">
         <v>3</v>
@@ -2727,7 +2679,7 @@
         <v>143</v>
       </c>
       <c r="B109" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -2738,7 +2690,7 @@
         <v>6</v>
       </c>
       <c r="B110" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C110">
         <v>5</v>
@@ -2749,7 +2701,7 @@
         <v>95</v>
       </c>
       <c r="B111" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C111">
         <v>3</v>
@@ -2760,7 +2712,7 @@
         <v>116</v>
       </c>
       <c r="B112" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C112">
         <v>3</v>
@@ -2771,7 +2723,7 @@
         <v>129</v>
       </c>
       <c r="B113" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C113">
         <v>0</v>
@@ -2782,7 +2734,7 @@
         <v>219</v>
       </c>
       <c r="B114" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C114">
         <v>6</v>
@@ -2793,7 +2745,7 @@
         <v>261</v>
       </c>
       <c r="B115" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C115">
         <v>3</v>
@@ -2804,7 +2756,7 @@
         <v>60</v>
       </c>
       <c r="B116" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C116">
         <v>3</v>
@@ -2815,7 +2767,7 @@
         <v>64</v>
       </c>
       <c r="B117" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C117">
         <v>0</v>
@@ -2826,7 +2778,7 @@
         <v>3</v>
       </c>
       <c r="B118" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C118">
         <v>4</v>
@@ -2837,7 +2789,7 @@
         <v>35</v>
       </c>
       <c r="B119" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C119">
         <v>9</v>
@@ -2848,7 +2800,7 @@
         <v>49</v>
       </c>
       <c r="B120" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C120">
         <v>3</v>
@@ -2859,7 +2811,7 @@
         <v>62</v>
       </c>
       <c r="B121" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C121">
         <v>5</v>
@@ -2870,7 +2822,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C122">
         <v>2</v>
@@ -2881,7 +2833,7 @@
         <v>126</v>
       </c>
       <c r="B123" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C123">
         <v>3</v>
@@ -2892,7 +2844,7 @@
         <v>151</v>
       </c>
       <c r="B124" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C124">
         <v>5</v>
@@ -2903,7 +2855,7 @@
         <v>175</v>
       </c>
       <c r="B125" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C125">
         <v>2</v>
@@ -2914,7 +2866,7 @@
         <v>173</v>
       </c>
       <c r="B126" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C126">
         <v>4</v>
@@ -2925,7 +2877,7 @@
         <v>186</v>
       </c>
       <c r="B127" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C127">
         <v>2</v>
@@ -2936,7 +2888,7 @@
         <v>196</v>
       </c>
       <c r="B128" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C128">
         <v>7</v>
@@ -2947,7 +2899,7 @@
         <v>213</v>
       </c>
       <c r="B129" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C129">
         <v>6</v>
@@ -2958,7 +2910,7 @@
         <v>183</v>
       </c>
       <c r="B130" t="s">
-        <v>338</v>
+        <v>351</v>
       </c>
       <c r="C130">
         <v>4</v>
@@ -2969,7 +2921,7 @@
         <v>153</v>
       </c>
       <c r="B131" t="s">
-        <v>329</v>
+        <v>351</v>
       </c>
       <c r="C131">
         <v>2</v>
@@ -2980,7 +2932,7 @@
         <v>18</v>
       </c>
       <c r="B132" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C132">
         <v>0</v>
@@ -2991,7 +2943,7 @@
         <v>184</v>
       </c>
       <c r="B133" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C133">
         <v>8</v>
@@ -3002,7 +2954,7 @@
         <v>16</v>
       </c>
       <c r="B134" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C134">
         <v>5</v>
@@ -3013,7 +2965,7 @@
         <v>254</v>
       </c>
       <c r="B135" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C135">
         <v>5</v>
@@ -3024,7 +2976,7 @@
         <v>94</v>
       </c>
       <c r="B136" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C136">
         <v>3</v>
@@ -3035,7 +2987,7 @@
         <v>163</v>
       </c>
       <c r="B137" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="C137">
         <v>4</v>
@@ -3046,7 +2998,7 @@
         <v>105</v>
       </c>
       <c r="B138" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C138">
         <v>1</v>
@@ -3057,7 +3009,7 @@
         <v>199</v>
       </c>
       <c r="B139" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C139">
         <v>6</v>
@@ -3068,7 +3020,7 @@
         <v>38</v>
       </c>
       <c r="B140" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C140">
         <v>4</v>
@@ -3079,7 +3031,7 @@
         <v>258</v>
       </c>
       <c r="B141" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="C141">
         <v>3</v>
@@ -3090,7 +3042,7 @@
         <v>26</v>
       </c>
       <c r="B142" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C142">
         <v>1</v>
@@ -3101,7 +3053,7 @@
         <v>100</v>
       </c>
       <c r="B143" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C143">
         <v>0</v>
@@ -3112,7 +3064,7 @@
         <v>96</v>
       </c>
       <c r="B144" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C144">
         <v>1</v>
@@ -3123,7 +3075,7 @@
         <v>156</v>
       </c>
       <c r="B145" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C145">
         <v>6</v>
@@ -3134,7 +3086,7 @@
         <v>236</v>
       </c>
       <c r="B146" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="C146">
         <v>1</v>
@@ -3145,7 +3097,7 @@
         <v>135</v>
       </c>
       <c r="B147" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="C147">
         <v>4</v>
@@ -3156,7 +3108,7 @@
         <v>140</v>
       </c>
       <c r="B148" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="C148">
         <v>2</v>
@@ -3167,7 +3119,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="C149">
         <v>5</v>
@@ -3178,7 +3130,7 @@
         <v>159</v>
       </c>
       <c r="B150" t="s">
-        <v>323</v>
+        <v>351</v>
       </c>
       <c r="C150">
         <v>3</v>
@@ -3189,7 +3141,7 @@
         <v>180</v>
       </c>
       <c r="B151" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="C151">
         <v>4</v>
@@ -3607,7 +3559,7 @@
         <v>84</v>
       </c>
       <c r="B189" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C189">
         <v>9</v>
@@ -3618,7 +3570,7 @@
         <v>160</v>
       </c>
       <c r="B190" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C190">
         <v>0</v>
@@ -3629,7 +3581,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C191">
         <v>0</v>
@@ -3640,7 +3592,7 @@
         <v>224</v>
       </c>
       <c r="B192" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C192">
         <v>7</v>
@@ -3651,7 +3603,7 @@
         <v>241</v>
       </c>
       <c r="B193" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="C193">
         <v>7</v>
@@ -3662,7 +3614,7 @@
         <v>203</v>
       </c>
       <c r="B194" t="s">
-        <v>341</v>
+        <v>351</v>
       </c>
       <c r="C194">
         <v>6</v>
@@ -3673,7 +3625,7 @@
         <v>11</v>
       </c>
       <c r="B195" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C195">
         <v>4</v>
@@ -3684,7 +3636,7 @@
         <v>251</v>
       </c>
       <c r="B196" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="C196">
         <v>4</v>
@@ -3695,7 +3647,7 @@
         <v>130</v>
       </c>
       <c r="B197" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C197">
         <v>4</v>
@@ -3706,7 +3658,7 @@
         <v>154</v>
       </c>
       <c r="B198" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="C198">
         <v>6</v>
@@ -3717,7 +3669,7 @@
         <v>167</v>
       </c>
       <c r="B199" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="C199">
         <v>3</v>
@@ -3728,7 +3680,7 @@
         <v>239</v>
       </c>
       <c r="B200" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="C200">
         <v>3</v>
@@ -3739,7 +3691,7 @@
         <v>259</v>
       </c>
       <c r="B201" t="s">
-        <v>330</v>
+        <v>351</v>
       </c>
       <c r="C201">
         <v>2</v>
@@ -3750,7 +3702,7 @@
         <v>169</v>
       </c>
       <c r="B202" t="s">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="C202">
         <v>5</v>
@@ -3761,7 +3713,7 @@
         <v>274</v>
       </c>
       <c r="B203" t="s">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="C203">
         <v>5</v>
@@ -3772,7 +3724,7 @@
         <v>162</v>
       </c>
       <c r="B204" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="C204">
         <v>4</v>
@@ -3783,7 +3735,7 @@
         <v>68</v>
       </c>
       <c r="B205" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="C205">
         <v>0</v>
@@ -3794,7 +3746,7 @@
         <v>231</v>
       </c>
       <c r="B206" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C206">
         <v>0</v>
@@ -3805,7 +3757,7 @@
         <v>108</v>
       </c>
       <c r="B207" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C207">
         <v>0</v>
@@ -3816,7 +3768,7 @@
         <v>138</v>
       </c>
       <c r="B208" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C208">
         <v>0</v>
@@ -3827,7 +3779,7 @@
         <v>146</v>
       </c>
       <c r="B209" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C209">
         <v>3</v>
@@ -3838,7 +3790,7 @@
         <v>168</v>
       </c>
       <c r="B210" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C210">
         <v>7</v>
@@ -3849,7 +3801,7 @@
         <v>31</v>
       </c>
       <c r="B211" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C211">
         <v>1</v>
@@ -3860,7 +3812,7 @@
         <v>32</v>
       </c>
       <c r="B212" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C212">
         <v>0</v>
@@ -3871,7 +3823,7 @@
         <v>36</v>
       </c>
       <c r="B213" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C213">
         <v>4</v>
@@ -3882,7 +3834,7 @@
         <v>54</v>
       </c>
       <c r="B214" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C214">
         <v>3</v>
@@ -3893,7 +3845,7 @@
         <v>273</v>
       </c>
       <c r="B215" t="s">
-        <v>361</v>
+        <v>351</v>
       </c>
       <c r="C215">
         <v>4</v>
@@ -3904,7 +3856,7 @@
         <v>266</v>
       </c>
       <c r="B216" t="s">
-        <v>358</v>
+        <v>341</v>
       </c>
       <c r="C216">
         <v>2</v>
@@ -3915,7 +3867,7 @@
         <v>226</v>
       </c>
       <c r="B217" t="s">
-        <v>347</v>
+        <v>334</v>
       </c>
       <c r="C217">
         <v>0</v>
@@ -3926,7 +3878,7 @@
         <v>134</v>
       </c>
       <c r="B218" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="C218">
         <v>5</v>
@@ -3937,7 +3889,7 @@
         <v>225</v>
       </c>
       <c r="B219" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="C219">
         <v>2</v>
@@ -3948,7 +3900,7 @@
         <v>242</v>
       </c>
       <c r="B220" t="s">
-        <v>346</v>
+        <v>333</v>
       </c>
       <c r="C220">
         <v>3</v>
@@ -3959,7 +3911,7 @@
         <v>145</v>
       </c>
       <c r="B221" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C221">
         <v>7</v>
@@ -3970,7 +3922,7 @@
         <v>222</v>
       </c>
       <c r="B222" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="C222">
         <v>4</v>
@@ -3981,7 +3933,7 @@
         <v>15</v>
       </c>
       <c r="B223" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C223">
         <v>3</v>
@@ -3992,7 +3944,7 @@
         <v>37</v>
       </c>
       <c r="B224" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C224">
         <v>3</v>
@@ -4003,7 +3955,7 @@
         <v>111</v>
       </c>
       <c r="B225" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C225">
         <v>5</v>
@@ -4014,7 +3966,7 @@
         <v>123</v>
       </c>
       <c r="B226" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C226">
         <v>3</v>
@@ -4025,7 +3977,7 @@
         <v>173</v>
       </c>
       <c r="B227" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C227">
         <v>2</v>
@@ -4036,7 +3988,7 @@
         <v>176</v>
       </c>
       <c r="B228" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C228">
         <v>3</v>
@@ -4047,7 +3999,7 @@
         <v>189</v>
       </c>
       <c r="B229" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C229">
         <v>0</v>
@@ -4058,7 +4010,7 @@
         <v>204</v>
       </c>
       <c r="B230" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C230">
         <v>0</v>
@@ -4069,7 +4021,7 @@
         <v>210</v>
       </c>
       <c r="B231" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C231">
         <v>5</v>
@@ -4080,7 +4032,7 @@
         <v>215</v>
       </c>
       <c r="B232" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C232">
         <v>4</v>
@@ -4091,7 +4043,7 @@
         <v>246</v>
       </c>
       <c r="B233" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C233">
         <v>1</v>
@@ -4102,7 +4054,7 @@
         <v>263</v>
       </c>
       <c r="B234" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C234">
         <v>4</v>
@@ -4113,7 +4065,7 @@
         <v>165</v>
       </c>
       <c r="B235" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C235">
         <v>0</v>
@@ -4124,7 +4076,7 @@
         <v>247</v>
       </c>
       <c r="B236" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="C236">
         <v>5</v>
@@ -4135,7 +4087,7 @@
         <v>206</v>
       </c>
       <c r="B237" t="s">
-        <v>342</v>
+        <v>330</v>
       </c>
       <c r="C237">
         <v>0</v>
@@ -4146,7 +4098,7 @@
         <v>72</v>
       </c>
       <c r="B238" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="C238">
         <v>0</v>
@@ -4157,7 +4109,7 @@
         <v>17</v>
       </c>
       <c r="B239" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C239">
         <v>6</v>
@@ -4168,7 +4120,7 @@
         <v>48</v>
       </c>
       <c r="B240" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C240">
         <v>4</v>
@@ -4179,7 +4131,7 @@
         <v>66</v>
       </c>
       <c r="B241" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C241">
         <v>4</v>
@@ -4190,7 +4142,7 @@
         <v>71</v>
       </c>
       <c r="B242" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C242">
         <v>12</v>
@@ -4201,7 +4153,7 @@
         <v>161</v>
       </c>
       <c r="B243" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C243">
         <v>1</v>
@@ -4212,7 +4164,7 @@
         <v>209</v>
       </c>
       <c r="B244" t="s">
-        <v>344</v>
+        <v>331</v>
       </c>
       <c r="C244">
         <v>0</v>
@@ -4223,7 +4175,7 @@
         <v>58</v>
       </c>
       <c r="B245" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C245">
         <v>3</v>
@@ -4234,7 +4186,7 @@
         <v>218</v>
       </c>
       <c r="B246" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="C246">
         <v>0</v>
@@ -4245,7 +4197,7 @@
         <v>267</v>
       </c>
       <c r="B247" t="s">
-        <v>359</v>
+        <v>342</v>
       </c>
       <c r="C247">
         <v>3</v>
@@ -4256,7 +4208,7 @@
         <v>20</v>
       </c>
       <c r="B248" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C248">
         <v>5</v>
@@ -4267,7 +4219,7 @@
         <v>171</v>
       </c>
       <c r="B249" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C249">
         <v>5</v>
@@ -4278,7 +4230,7 @@
         <v>34</v>
       </c>
       <c r="B250" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C250">
         <v>2</v>
@@ -4289,7 +4241,7 @@
         <v>41</v>
       </c>
       <c r="B251" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C251">
         <v>3</v>
@@ -4300,7 +4252,7 @@
         <v>50</v>
       </c>
       <c r="B252" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C252">
         <v>5</v>
@@ -4311,7 +4263,7 @@
         <v>51</v>
       </c>
       <c r="B253" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C253">
         <v>11</v>
@@ -4322,7 +4274,7 @@
         <v>59</v>
       </c>
       <c r="B254" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C254">
         <v>7</v>
@@ -4333,7 +4285,7 @@
         <v>75</v>
       </c>
       <c r="B255" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C255">
         <v>3</v>
@@ -4344,7 +4296,7 @@
         <v>81</v>
       </c>
       <c r="B256" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C256">
         <v>2</v>
@@ -4355,7 +4307,7 @@
         <v>82</v>
       </c>
       <c r="B257" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C257">
         <v>3</v>
@@ -4366,7 +4318,7 @@
         <v>85</v>
       </c>
       <c r="B258" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C258">
         <v>3</v>
@@ -4377,7 +4329,7 @@
         <v>93</v>
       </c>
       <c r="B259" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C259">
         <v>10</v>
@@ -4388,7 +4340,7 @@
         <v>97</v>
       </c>
       <c r="B260" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C260">
         <v>4</v>
@@ -4399,7 +4351,7 @@
         <v>102</v>
       </c>
       <c r="B261" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C261">
         <v>0</v>
@@ -4410,7 +4362,7 @@
         <v>104</v>
       </c>
       <c r="B262" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C262">
         <v>8</v>
@@ -4421,7 +4373,7 @@
         <v>166</v>
       </c>
       <c r="B263" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C263">
         <v>0</v>
@@ -4432,7 +4384,7 @@
         <v>170</v>
       </c>
       <c r="B264" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C264">
         <v>9</v>
@@ -4443,7 +4395,7 @@
         <v>179</v>
       </c>
       <c r="B265" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C265">
         <v>2</v>
@@ -4454,7 +4406,7 @@
         <v>192</v>
       </c>
       <c r="B266" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C266">
         <v>2</v>
@@ -4465,7 +4417,7 @@
         <v>265</v>
       </c>
       <c r="B267" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C267">
         <v>4</v>
@@ -4476,7 +4428,7 @@
         <v>271</v>
       </c>
       <c r="B268" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C268">
         <v>3</v>
@@ -4487,7 +4439,7 @@
         <v>194</v>
       </c>
       <c r="B269" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C269">
         <v>3</v>
@@ -4498,7 +4450,7 @@
         <v>208</v>
       </c>
       <c r="B270" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C270">
         <v>3</v>
@@ -4509,7 +4461,7 @@
         <v>212</v>
       </c>
       <c r="B271" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C271">
         <v>5</v>
@@ -4520,7 +4472,7 @@
         <v>46</v>
       </c>
       <c r="B272" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C272">
         <v>6</v>
@@ -4531,7 +4483,7 @@
         <v>73</v>
       </c>
       <c r="B273" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C273">
         <v>1</v>
@@ -4542,7 +4494,7 @@
         <v>152</v>
       </c>
       <c r="B274" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C274">
         <v>4</v>
@@ -4553,7 +4505,7 @@
         <v>177</v>
       </c>
       <c r="B275" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C275">
         <v>5</v>
@@ -4564,7 +4516,7 @@
         <v>243</v>
       </c>
       <c r="B276" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="C276">
         <v>0</v>

</xml_diff>